<commit_message>
[FEATURE] Penambahan Report Tahunan
</commit_message>
<xml_diff>
--- a/.excel/daily_transactions_2024-03-08.xlsx
+++ b/.excel/daily_transactions_2024-03-08.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Transaction_id</t>
   </si>
@@ -45,61 +45,7 @@
     <t>Updated_at</t>
   </si>
   <si>
-    <t>Jumlah</t>
-  </si>
-  <si>
-    <t>00000000-0000-0000-0000-000000000000</t>
-  </si>
-  <si>
-    <t>0001-01-01T00:00:00Z</t>
-  </si>
-  <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>12345678-1234-1234-1234-123456789012</t>
-  </si>
-  <si>
-    <t>11111111-1111-1111-1111-111111111111</t>
-  </si>
-  <si>
-    <t>77777777-7777-7777-7777-777777777777</t>
-  </si>
-  <si>
-    <t>2024-03-05T00:00:00Z</t>
-  </si>
-  <si>
-    <t>Meeting with clients</t>
-  </si>
-  <si>
-    <t>2024-03-07T00:00:00Z</t>
-  </si>
-  <si>
-    <t>2024-03-06T09:51:37.808009Z</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>23456789-2345-2345-2345-234567890123</t>
-  </si>
-  <si>
-    <t>22222222-2222-2222-2222-222222222222</t>
-  </si>
-  <si>
-    <t>88888888-8888-8888-8888-888888888888</t>
-  </si>
-  <si>
-    <t>2024-03-08T00:00:00Z</t>
-  </si>
-  <si>
-    <t>Team building event</t>
-  </si>
-  <si>
-    <t>2024-03-10T00:00:00Z</t>
+    <t>Jumlah_Transaksi</t>
   </si>
 </sst>
 </file>
@@ -466,7 +412,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -518,100 +464,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s"/>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>